<commit_message>
update the get orders
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsfile/data.xlsx
+++ b/src/main/resources/xlsfile/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468D00E0-6E40-4AFF-93F3-C7381A7A187B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051219B1-B53D-464D-A3D3-CFBC5461FEAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="3" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>t001,t002</t>
   </si>
   <si>
-    <t>t003,t004,t005</t>
-  </si>
-  <si>
     <t>p0006</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Don't use this</t>
+  </si>
+  <si>
+    <t>t003,t004,t005,t006</t>
   </si>
 </sst>
 </file>
@@ -564,13 +564,13 @@
       <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -592,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -603,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -626,20 +626,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B2F33-3E03-494D-9F30-1DF0D32D4E4D}">
   <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -656,7 +656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -673,7 +673,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -690,7 +690,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -707,7 +707,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -724,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -741,15 +741,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>48</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
@@ -772,17 +772,17 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>30</v>
       </c>
@@ -793,7 +793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -804,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -815,7 +815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>35</v>
       </c>
@@ -826,7 +826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -837,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -871,16 +871,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5A8D0-6A69-4317-BF67-BDCA8742CFBC}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>40</v>
       </c>
@@ -888,7 +888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -896,12 +896,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>